<commit_message>
Update of the test performance reports.
</commit_message>
<xml_diff>
--- a/test/PyBWE_Report_test_performances_white_noise.xlsx
+++ b/test/PyBWE_Report_test_performances_white_noise.xlsx
@@ -489,19 +489,19 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>86.5</v>
+        <v>100</v>
       </c>
       <c r="C4" t="n">
-        <v>97.40000000000001</v>
+        <v>100</v>
       </c>
       <c r="D4" t="n">
-        <v>97.09999999999999</v>
+        <v>100</v>
       </c>
       <c r="E4" t="n">
-        <v>93.8</v>
+        <v>100</v>
       </c>
       <c r="F4" t="n">
-        <v>59.5</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5">
@@ -509,19 +509,19 @@
         <v>14</v>
       </c>
       <c r="B5" t="n">
-        <v>93.8</v>
+        <v>100</v>
       </c>
       <c r="C5" t="n">
         <v>100</v>
       </c>
       <c r="D5" t="n">
-        <v>98.8</v>
+        <v>100</v>
       </c>
       <c r="E5" t="n">
-        <v>98.40000000000001</v>
+        <v>100</v>
       </c>
       <c r="F5" t="n">
-        <v>74.09999999999999</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6">
@@ -529,19 +529,19 @@
         <v>20</v>
       </c>
       <c r="B6" t="n">
-        <v>91.3</v>
+        <v>100</v>
       </c>
       <c r="C6" t="n">
         <v>100</v>
       </c>
       <c r="D6" t="n">
-        <v>99.2</v>
+        <v>100</v>
       </c>
       <c r="E6" t="n">
-        <v>98.8</v>
+        <v>100</v>
       </c>
       <c r="F6" t="n">
-        <v>89.3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7">
@@ -549,7 +549,7 @@
         <v>40</v>
       </c>
       <c r="B7" t="n">
-        <v>40.5</v>
+        <v>100</v>
       </c>
       <c r="C7" t="n">
         <v>100</v>
@@ -558,10 +558,10 @@
         <v>100</v>
       </c>
       <c r="E7" t="n">
-        <v>93.5</v>
+        <v>100</v>
       </c>
       <c r="F7" t="n">
-        <v>94.59999999999999</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8">
@@ -569,13 +569,13 @@
         <v>60</v>
       </c>
       <c r="B8" t="n">
-        <v>56.3</v>
+        <v>100</v>
       </c>
       <c r="C8" t="n">
         <v>100</v>
       </c>
       <c r="D8" t="n">
-        <v>99.7</v>
+        <v>100</v>
       </c>
       <c r="E8" t="n">
         <v>100</v>
@@ -648,19 +648,19 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.02376854380397079</v>
+        <v>0.02365783452653334</v>
       </c>
       <c r="C4" t="n">
-        <v>0.001560723470351691</v>
+        <v>0.001543287327478072</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0046042350460194</v>
+        <v>0.004641670972027444</v>
       </c>
       <c r="E4" t="n">
-        <v>0.005593989501266892</v>
+        <v>0.005618864860875331</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.004542317923552986</v>
+        <v>-0.004364159716584307</v>
       </c>
     </row>
     <row r="5">
@@ -668,19 +668,19 @@
         <v>14</v>
       </c>
       <c r="B5" t="n">
-        <v>0.02186500518295674</v>
+        <v>0.02181784633552293</v>
       </c>
       <c r="C5" t="n">
         <v>0.001363938298029429</v>
       </c>
       <c r="D5" t="n">
-        <v>0.004688115082667425</v>
+        <v>0.004694811425197448</v>
       </c>
       <c r="E5" t="n">
-        <v>0.005025301120233881</v>
+        <v>0.005029891504908117</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.003081441091160276</v>
+        <v>-0.00288508377002</v>
       </c>
     </row>
     <row r="6">
@@ -688,19 +688,19 @@
         <v>20</v>
       </c>
       <c r="B6" t="n">
-        <v>0.01939255650477833</v>
+        <v>0.01946638128275146</v>
       </c>
       <c r="C6" t="n">
         <v>0.001062809063399571</v>
       </c>
       <c r="D6" t="n">
-        <v>0.00430645399374793</v>
+        <v>0.004305114768617639</v>
       </c>
       <c r="E6" t="n">
-        <v>0.004165328244790331</v>
+        <v>0.004161930769798526</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.001777864541599607</v>
+        <v>-0.001764705882353011</v>
       </c>
     </row>
     <row r="7">
@@ -708,7 +708,7 @@
         <v>40</v>
       </c>
       <c r="B7" t="n">
-        <v>0.01703304603592436</v>
+        <v>0.01666765074913267</v>
       </c>
       <c r="C7" t="n">
         <v>-0.0006177577681009469</v>
@@ -717,10 +717,10 @@
         <v>0.002405343567791018</v>
       </c>
       <c r="E7" t="n">
-        <v>0.00284477454183926</v>
+        <v>0.00287327478042663</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.0005767555456454263</v>
+        <v>-0.0006044726548085195</v>
       </c>
     </row>
     <row r="8">
@@ -728,13 +728,13 @@
         <v>60</v>
       </c>
       <c r="B8" t="n">
-        <v>0.01154372256110866</v>
+        <v>0.01181858439737245</v>
       </c>
       <c r="C8" t="n">
         <v>0.002623809875267612</v>
       </c>
       <c r="D8" t="n">
-        <v>0.003079706312087092</v>
+        <v>0.003082884345708216</v>
       </c>
       <c r="E8" t="n">
         <v>0.004066720791202322</v>
@@ -807,19 +807,19 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.001946364517851141</v>
+        <v>0.002035967391253168</v>
       </c>
       <c r="C4" t="n">
-        <v>0.002482288172583826</v>
+        <v>0.002490319006590181</v>
       </c>
       <c r="D4" t="n">
-        <v>0.002021233676331818</v>
+        <v>0.002043143839331984</v>
       </c>
       <c r="E4" t="n">
-        <v>0.001861136404846659</v>
+        <v>0.001880883832005884</v>
       </c>
       <c r="F4" t="n">
-        <v>0.002481883479813886</v>
+        <v>0.002546193042046593</v>
       </c>
     </row>
     <row r="5">
@@ -827,19 +827,19 @@
         <v>14</v>
       </c>
       <c r="B5" t="n">
-        <v>0.001690323918718363</v>
+        <v>0.001704259925763946</v>
       </c>
       <c r="C5" t="n">
         <v>0.001421576098366335</v>
       </c>
       <c r="D5" t="n">
-        <v>0.001280130634611951</v>
+        <v>0.001279636429058974</v>
       </c>
       <c r="E5" t="n">
-        <v>0.001342191739347798</v>
+        <v>0.001342780772921734</v>
       </c>
       <c r="F5" t="n">
-        <v>0.001536071810846572</v>
+        <v>0.001592907613271836</v>
       </c>
     </row>
     <row r="6">
@@ -847,19 +847,19 @@
         <v>20</v>
       </c>
       <c r="B6" t="n">
-        <v>0.001780855355541221</v>
+        <v>0.001788633010541431</v>
       </c>
       <c r="C6" t="n">
         <v>0.001324660445840111</v>
       </c>
       <c r="D6" t="n">
-        <v>0.001551920921239779</v>
+        <v>0.001548941093028976</v>
       </c>
       <c r="E6" t="n">
-        <v>0.001373252732818081</v>
+        <v>0.001370562969376771</v>
       </c>
       <c r="F6" t="n">
-        <v>0.001442543968384869</v>
+        <v>0.001451599173634971</v>
       </c>
     </row>
     <row r="7">
@@ -867,7 +867,7 @@
         <v>40</v>
       </c>
       <c r="B7" t="n">
-        <v>0.00107961527256598</v>
+        <v>0.001161869472433352</v>
       </c>
       <c r="C7" t="n">
         <v>0.001163741464175242</v>
@@ -876,10 +876,10 @@
         <v>0.002229533125642799</v>
       </c>
       <c r="E7" t="n">
-        <v>0.001222950907525686</v>
+        <v>0.001225785198558041</v>
       </c>
       <c r="F7" t="n">
-        <v>0.001317752991108748</v>
+        <v>0.001359645151408854</v>
       </c>
     </row>
     <row r="8">
@@ -887,13 +887,13 @@
         <v>60</v>
       </c>
       <c r="B8" t="n">
-        <v>0.001206707301210268</v>
+        <v>0.001249771922356871</v>
       </c>
       <c r="C8" t="n">
         <v>0.0009973941291286348</v>
       </c>
       <c r="D8" t="n">
-        <v>0.001562972237790004</v>
+        <v>0.00156170102840523</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -966,19 +966,19 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>-26.64756218761986</v>
+        <v>-26.54589195190782</v>
       </c>
       <c r="C4" t="n">
-        <v>-4.656762526144954</v>
+        <v>-4.614615457333819</v>
       </c>
       <c r="D4" t="n">
-        <v>-9.198372304141229</v>
+        <v>-9.156226171518295</v>
       </c>
       <c r="E4" t="n">
-        <v>-6.18133474223607</v>
+        <v>-6.116429325715128</v>
       </c>
       <c r="F4" t="n">
-        <v>-2.257412565841321</v>
+        <v>-2.310349471226028</v>
       </c>
     </row>
     <row r="5">
@@ -986,19 +986,19 @@
         <v>14</v>
       </c>
       <c r="B5" t="n">
-        <v>-24.23240452327419</v>
+        <v>-24.21109122750564</v>
       </c>
       <c r="C5" t="n">
         <v>-2.001205553204233</v>
       </c>
       <c r="D5" t="n">
-        <v>-8.116124460687088</v>
+        <v>-8.054217653056249</v>
       </c>
       <c r="E5" t="n">
-        <v>-4.803500542239189</v>
+        <v>-4.744366658482702</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.7720884595229529</v>
+        <v>-0.5939367701619458</v>
       </c>
     </row>
     <row r="6">
@@ -1006,19 +1006,19 @@
         <v>20</v>
       </c>
       <c r="B6" t="n">
-        <v>-22.29206988924489</v>
+        <v>-22.30166806259818</v>
       </c>
       <c r="C6" t="n">
         <v>-1.818206249692174</v>
       </c>
       <c r="D6" t="n">
-        <v>-7.658861671306038</v>
+        <v>-7.602445697231851</v>
       </c>
       <c r="E6" t="n">
-        <v>-4.498832146429911</v>
+        <v>-4.452177570026453</v>
       </c>
       <c r="F6" t="n">
-        <v>0.4687892588818198</v>
+        <v>0.7389267850343705</v>
       </c>
     </row>
     <row r="7">
@@ -1026,7 +1026,7 @@
         <v>40</v>
       </c>
       <c r="B7" t="n">
-        <v>-17.43294715505795</v>
+        <v>-18.04829467257114</v>
       </c>
       <c r="C7" t="n">
         <v>-0.1591731907007712</v>
@@ -1035,10 +1035,10 @@
         <v>-4.150066273483676</v>
       </c>
       <c r="E7" t="n">
-        <v>0.004649680835465402</v>
+        <v>0.4039858422133276</v>
       </c>
       <c r="F7" t="n">
-        <v>2.188356444631826</v>
+        <v>2.224410226504793</v>
       </c>
     </row>
     <row r="8">
@@ -1046,13 +1046,13 @@
         <v>60</v>
       </c>
       <c r="B8" t="n">
-        <v>-10.26727057546294</v>
+        <v>-10.99568223481967</v>
       </c>
       <c r="C8" t="n">
         <v>-3.003623810105132</v>
       </c>
       <c r="D8" t="n">
-        <v>-2.155568810892131</v>
+        <v>-2.149683673259656</v>
       </c>
       <c r="E8" t="n">
         <v>-0.008612120923525559</v>
@@ -1125,19 +1125,19 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>3.262487507281837</v>
+        <v>3.334744370426787</v>
       </c>
       <c r="C4" t="n">
-        <v>5.268274408494276</v>
+        <v>5.299820319418025</v>
       </c>
       <c r="D4" t="n">
-        <v>3.700199915103403</v>
+        <v>3.737126619954745</v>
       </c>
       <c r="E4" t="n">
-        <v>3.340485886755907</v>
+        <v>3.396576810952055</v>
       </c>
       <c r="F4" t="n">
-        <v>3.795378820647012</v>
+        <v>5.016290421391401</v>
       </c>
     </row>
     <row r="5">
@@ -1145,19 +1145,19 @@
         <v>14</v>
       </c>
       <c r="B5" t="n">
-        <v>2.520213317435309</v>
+        <v>2.526736109056072</v>
       </c>
       <c r="C5" t="n">
         <v>3.368264599626112</v>
       </c>
       <c r="D5" t="n">
-        <v>2.458583834515497</v>
+        <v>2.519867400252476</v>
       </c>
       <c r="E5" t="n">
-        <v>2.242363103740262</v>
+        <v>2.289296289438998</v>
       </c>
       <c r="F5" t="n">
-        <v>2.824430018777426</v>
+        <v>3.303014865323734</v>
       </c>
     </row>
     <row r="6">
@@ -1165,19 +1165,19 @@
         <v>20</v>
       </c>
       <c r="B6" t="n">
-        <v>2.728212559791231</v>
+        <v>2.847031525659731</v>
       </c>
       <c r="C6" t="n">
         <v>3.03711430495359</v>
       </c>
       <c r="D6" t="n">
-        <v>2.913225543657266</v>
+        <v>2.969924482433771</v>
       </c>
       <c r="E6" t="n">
-        <v>2.433867087110785</v>
+        <v>2.462110949048284</v>
       </c>
       <c r="F6" t="n">
-        <v>3.172668596474179</v>
+        <v>3.410486569297024</v>
       </c>
     </row>
     <row r="7">
@@ -1185,7 +1185,7 @@
         <v>40</v>
       </c>
       <c r="B7" t="n">
-        <v>1.227536969172887</v>
+        <v>1.568207772039397</v>
       </c>
       <c r="C7" t="n">
         <v>1.945205081730048</v>
@@ -1194,10 +1194,10 @@
         <v>2.547513087256319</v>
       </c>
       <c r="E7" t="n">
-        <v>2.892062961318839</v>
+        <v>3.226978287566372</v>
       </c>
       <c r="F7" t="n">
-        <v>2.005277911313566</v>
+        <v>2.006297947669716</v>
       </c>
     </row>
     <row r="8">
@@ -1205,13 +1205,13 @@
         <v>60</v>
       </c>
       <c r="B8" t="n">
-        <v>1.072920113234682</v>
+        <v>1.365072671008647</v>
       </c>
       <c r="C8" t="n">
         <v>1.30121483615577</v>
       </c>
       <c r="D8" t="n">
-        <v>1.163396642390335</v>
+        <v>1.166648896344525</v>
       </c>
       <c r="E8" t="n">
         <v>0.915181901083999</v>
@@ -1284,19 +1284,19 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>-27.01372802044695</v>
+        <v>-26.86031049084387</v>
       </c>
       <c r="C4" t="n">
-        <v>-4.666124182318693</v>
+        <v>-4.647840414730961</v>
       </c>
       <c r="D4" t="n">
-        <v>-9.001259551282951</v>
+        <v>-9.00760275339627</v>
       </c>
       <c r="E4" t="n">
-        <v>-6.369147971002324</v>
+        <v>-6.325938980223003</v>
       </c>
       <c r="F4" t="n">
-        <v>-2.479666943801193</v>
+        <v>-3.230061096220323</v>
       </c>
     </row>
     <row r="5">
@@ -1304,19 +1304,19 @@
         <v>14</v>
       </c>
       <c r="B5" t="n">
-        <v>-23.66039152345261</v>
+        <v>-23.51424401310565</v>
       </c>
       <c r="C5" t="n">
         <v>-2.492601189440442</v>
       </c>
       <c r="D5" t="n">
-        <v>-8.290898289462707</v>
+        <v>-8.250225357458735</v>
       </c>
       <c r="E5" t="n">
-        <v>-5.060043449487075</v>
+        <v>-4.994416566227185</v>
       </c>
       <c r="F5" t="n">
-        <v>-1.236673886669486</v>
+        <v>-1.659610840162146</v>
       </c>
     </row>
     <row r="6">
@@ -1324,19 +1324,19 @@
         <v>20</v>
       </c>
       <c r="B6" t="n">
-        <v>-20.94343557566909</v>
+        <v>-20.86382596236752</v>
       </c>
       <c r="C6" t="n">
         <v>-1.400640112737667</v>
       </c>
       <c r="D6" t="n">
-        <v>-8.607903971852423</v>
+        <v>-8.536472800898901</v>
       </c>
       <c r="E6" t="n">
-        <v>-4.247351618695584</v>
+        <v>-4.179023357988734</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.1216653528896362</v>
+        <v>-0.021752606694643</v>
       </c>
     </row>
     <row r="7">
@@ -1344,7 +1344,7 @@
         <v>40</v>
       </c>
       <c r="B7" t="n">
-        <v>-14.45437904807576</v>
+        <v>-14.16240271748426</v>
       </c>
       <c r="C7" t="n">
         <v>2.998894532145355</v>
@@ -1353,10 +1353,10 @@
         <v>-7.519589438072102</v>
       </c>
       <c r="E7" t="n">
-        <v>0.07342204223185372</v>
+        <v>0.1024409273591615</v>
       </c>
       <c r="F7" t="n">
-        <v>5.069739588313046</v>
+        <v>5.208189141637962</v>
       </c>
     </row>
     <row r="8">
@@ -1364,13 +1364,13 @@
         <v>60</v>
       </c>
       <c r="B8" t="n">
-        <v>-12.09148265904057</v>
+        <v>-10.53113940143941</v>
       </c>
       <c r="C8" t="n">
         <v>-0.9133055584102008</v>
       </c>
       <c r="D8" t="n">
-        <v>-2.786411201170754</v>
+        <v>-2.776433776219893</v>
       </c>
       <c r="E8" t="n">
         <v>-4.814863765555236</v>
@@ -1443,19 +1443,19 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>3.390993063544938</v>
+        <v>3.452821354779885</v>
       </c>
       <c r="C4" t="n">
-        <v>5.062219323552082</v>
+        <v>5.059483158385259</v>
       </c>
       <c r="D4" t="n">
-        <v>3.656626761086554</v>
+        <v>3.680676563626293</v>
       </c>
       <c r="E4" t="n">
-        <v>3.175595329831998</v>
+        <v>3.211778697013214</v>
       </c>
       <c r="F4" t="n">
-        <v>3.911784680551411</v>
+        <v>5.182582469648143</v>
       </c>
     </row>
     <row r="5">
@@ -1463,19 +1463,19 @@
         <v>14</v>
       </c>
       <c r="B5" t="n">
-        <v>2.304449385876633</v>
+        <v>2.407673343220441</v>
       </c>
       <c r="C5" t="n">
         <v>3.409468904303833</v>
       </c>
       <c r="D5" t="n">
-        <v>2.621616320668644</v>
+        <v>2.666157798265959</v>
       </c>
       <c r="E5" t="n">
-        <v>2.210028348118065</v>
+        <v>2.266231230746703</v>
       </c>
       <c r="F5" t="n">
-        <v>2.987531884742659</v>
+        <v>3.724977976817463</v>
       </c>
     </row>
     <row r="6">
@@ -1483,19 +1483,19 @@
         <v>20</v>
       </c>
       <c r="B6" t="n">
-        <v>2.420474262901875</v>
+        <v>2.508002765111691</v>
       </c>
       <c r="C6" t="n">
         <v>3.091345706682579</v>
       </c>
       <c r="D6" t="n">
-        <v>3.046472189716187</v>
+        <v>3.139726948013384</v>
       </c>
       <c r="E6" t="n">
-        <v>2.273420640738195</v>
+        <v>2.353839641458567</v>
       </c>
       <c r="F6" t="n">
-        <v>3.20323237263903</v>
+        <v>3.474467643659124</v>
       </c>
     </row>
     <row r="7">
@@ -1503,7 +1503,7 @@
         <v>40</v>
       </c>
       <c r="B7" t="n">
-        <v>1.269351306598816</v>
+        <v>1.333850090809651</v>
       </c>
       <c r="C7" t="n">
         <v>2.3478139699096</v>
@@ -1512,10 +1512,10 @@
         <v>3.485736414373884</v>
       </c>
       <c r="E7" t="n">
-        <v>1.47847057653104</v>
+        <v>1.455138661921824</v>
       </c>
       <c r="F7" t="n">
-        <v>2.482206809000952</v>
+        <v>2.510831843449406</v>
       </c>
     </row>
     <row r="8">
@@ -1523,13 +1523,13 @@
         <v>60</v>
       </c>
       <c r="B8" t="n">
-        <v>1.936741547510429</v>
+        <v>2.552597245652156</v>
       </c>
       <c r="C8" t="n">
         <v>0.8385610884808548</v>
       </c>
       <c r="D8" t="n">
-        <v>2.293734049259941</v>
+        <v>2.297891957737512</v>
       </c>
       <c r="E8" t="n">
         <v>0.8156598424822077</v>

</xml_diff>